<commit_message>
Der erste Punkt des Temperaturprofils ist immer bei Raumtemperatur
</commit_message>
<xml_diff>
--- a/app/webui/models/tests/profile.xlsx
+++ b/app/webui/models/tests/profile.xlsx
@@ -11,12 +11,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Zeitstempel [Minuten]</t>
   </si>
   <si>
     <t>Temperatur [°C]</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Aufheizen 1</t>
+  </si>
+  <si>
+    <t>Aufheizen 2</t>
+  </si>
+  <si>
+    <t>Aufheizen 3</t>
+  </si>
+  <si>
+    <t>Halten</t>
+  </si>
+  <si>
+    <t>Abkühlen 1</t>
+  </si>
+  <si>
+    <t>Abkühlen 2</t>
   </si>
 </sst>
 </file>
@@ -86,61 +107,74 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="B2" s="1">
-        <v>20.0</v>
+        <v>30.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>0.5</v>
+        <v>5.0</v>
       </c>
       <c r="B3" s="1">
-        <v>30.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="B4" s="1">
-        <v>50.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>15.0</v>
+        <v>20.0</v>
       </c>
       <c r="B5" s="1">
         <v>60.0</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="B6" s="1">
-        <v>60.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>30.0</v>
+        <v>60.0</v>
       </c>
       <c r="B7" s="1">
-        <v>50.0</v>
+        <v>20.0</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20.0</v>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>